<commit_message>
Aggiunta funzionalità di selezione distanza
Aggiunta la funzionalità di selezione distanza attraverso scelta dell’utente. Ciò è stato realizzato attraverso il Design Strategy. Modificati di conseguenza i metodi evaluate e run del classificatore, che ora prende in input la scelta dell’utente. Aggiornati i test sulla base delle modifiche apportate. Aggiornato README.md con la funzionalità aggiunta.
</commit_message>
<xml_diff>
--- a/output/model_performance.xlsx
+++ b/output/model_performance.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9441860465116279</v>
+        <v>0.932514619883041</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.05581395348837209</v>
+        <v>0.06748538011695907</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9855595667870036</v>
+        <v>0.9190577399929153</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.869281045751634</v>
+        <v>0.9586776859504132</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9255961597085058</v>
+        <v>0.9386586959226578</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.962046671857672</v>
+        <v>0.952203097417026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>